<commit_message>
Some more EDA for residential sales, created tibble of the time series
</commit_message>
<xml_diff>
--- a/Energy_Data_Dictionary_2.xlsx
+++ b/Energy_Data_Dictionary_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sofia/Desktop/Education/UNIPD/Fall 2023/Business Economic and Financial Data/project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban\Documents\GitHub\business\business_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436F11BC-74FA-7F46-A2AC-FC8CDD1E294B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175639F2-B8E2-4333-A80F-CE7D695681C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="1060" windowWidth="27920" windowHeight="17500" xr2:uid="{0CF4C3A6-E06D-554F-B889-D0605F8E8A88}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{0CF4C3A6-E06D-554F-B889-D0605F8E8A88}"/>
   </bookViews>
   <sheets>
     <sheet name="Features description" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="141">
   <si>
     <t xml:space="preserve">DATE                                            </t>
   </si>
@@ -168,18 +168,6 @@
     <t>Energy generation (in MWh) from solar, thermal, and photovoltaic source</t>
   </si>
   <si>
-    <t>Combined Heat and Power, Commercial Power used to produce energy</t>
-  </si>
-  <si>
-    <t>Combined Heat and Power, Electric Power used to produce energy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electric Generators, Independent Power Producers used to produce energy </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electric Generators, Electric Utilities used to produce energy </t>
-  </si>
-  <si>
     <t>Column Number</t>
   </si>
   <si>
@@ -192,9 +180,6 @@
     <t>MWh</t>
   </si>
   <si>
-    <t>Thousand dollars</t>
-  </si>
-  <si>
     <t>Count</t>
   </si>
   <si>
@@ -228,52 +213,34 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Revenue (in thousand dollars) of residential electricity</t>
-  </si>
-  <si>
     <t>Sales (in MWh) of residential electricity</t>
   </si>
   <si>
     <t>Count of customers of residential electricity</t>
   </si>
   <si>
-    <t>Revenue (in thousand dollars) of commercial electricity</t>
-  </si>
-  <si>
     <t>Sales (in MWh) of commercial electricity</t>
   </si>
   <si>
     <t>Count of customers of commercial electricity</t>
   </si>
   <si>
-    <t>Revenue (in thousand dollars) of industrial electricity</t>
-  </si>
-  <si>
     <t>Sales (in MWh) of industrial electricity</t>
   </si>
   <si>
     <t>Count of customers of industrial electricity</t>
   </si>
   <si>
-    <t>Revenue (in thousand dollars) of transportation electricity</t>
-  </si>
-  <si>
     <t>Sales (in MWh) of transportation electricity</t>
   </si>
   <si>
     <t>Count of customers of transportation electricity</t>
   </si>
   <si>
-    <t>Revenue (in thousand dollars) of other electricity</t>
-  </si>
-  <si>
     <t>Sales (in MWh) of other electricity</t>
   </si>
   <si>
     <t>Count of customers of other electricity</t>
-  </si>
-  <si>
-    <t>Revenue (in thousand dollars) of total electricity</t>
   </si>
   <si>
     <t>Sales (in MWh) of total electricity</t>
@@ -577,12 +544,51 @@
   <si>
     <t>Average Price (in cents/KWh) of total electricity</t>
   </si>
+  <si>
+    <t>Electric Generators, Type of producer: Independent Power Producers</t>
+  </si>
+  <si>
+    <t>Electric Generators, Type of producer: Electric Utilities</t>
+  </si>
+  <si>
+    <t>Combined heat and power (CHP), also called cogeneration, is an efficient approach to generating electric power and useful thermal energy for heating or cooling from a single fuel source. Instead of purchasing electricity from the grid and producing heat in an on-site furnace or boiler, a CHP generator provides both energy services in one energy-efficient step. CHP plants can be found in three sectors: the electric power sector (plants whose primary purpose is to produce electricity for public sale); and the industrial and commercial sectors (where the CHP facility is usually intended to provide electricity and steam to the host facility, such as a factory). More than 85% of all generating capacity sited at industrial and commercial facilities uses CHP technology.</t>
+  </si>
+  <si>
+    <t>Combined Heat and Power (cogeneration), Type of producer: Commercial Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combined Heat and Power (cogeneration), Type of producer: Electric Power </t>
+  </si>
+  <si>
+    <t>Thousand dollars</t>
+  </si>
+  <si>
+    <t>Revenue (in Thousand dollars) of residential electricity</t>
+  </si>
+  <si>
+    <t>Revenue (in Thousand dollars) of commercial electricity</t>
+  </si>
+  <si>
+    <t>Revenue (in Thousand dollars) of industrial electricity</t>
+  </si>
+  <si>
+    <t>Revenue (in Thousand dollars) of transportation electricity</t>
+  </si>
+  <si>
+    <t>Revenue (in Thousand dollars) of other electricity</t>
+  </si>
+  <si>
+    <t>Revenue (in Thousand dollars) of total electricity</t>
+  </si>
+  <si>
+    <t>e.g. 10 cent/kwh = 100 dollars/MWh</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -638,6 +644,12 @@
       <vertAlign val="superscript"/>
       <sz val="6"/>
       <color rgb="FF3366CC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -719,7 +731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -739,12 +751,16 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1062,40 +1078,40 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="64.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="64.375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="99" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
         <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1106,7 +1122,7 @@
         <v>36</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>36</v>
@@ -1115,7 +1131,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="72" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1126,16 +1142,19 @@
         <v>38</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1146,16 +1165,16 @@
         <v>38</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1166,16 +1185,16 @@
         <v>38</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1186,19 +1205,19 @@
         <v>38</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>45</v>
+        <v>128</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -1209,16 +1228,16 @@
         <v>38</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -1229,16 +1248,16 @@
         <v>38</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1249,16 +1268,16 @@
         <v>38</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1269,16 +1288,16 @@
         <v>38</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1289,16 +1308,16 @@
         <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>51</v>
+        <v>133</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1309,16 +1328,16 @@
         <v>38</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1329,16 +1348,16 @@
         <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1349,16 +1368,19 @@
         <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1369,16 +1391,16 @@
         <v>38</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>51</v>
+        <v>133</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1389,16 +1411,16 @@
         <v>38</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1409,16 +1431,16 @@
         <v>38</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1429,16 +1451,16 @@
         <v>38</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1449,16 +1471,16 @@
         <v>38</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>51</v>
+        <v>133</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1469,16 +1491,16 @@
         <v>38</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1489,16 +1511,16 @@
         <v>38</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1509,16 +1531,16 @@
         <v>38</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1529,16 +1551,16 @@
         <v>38</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>51</v>
+        <v>133</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1549,16 +1571,16 @@
         <v>38</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1569,16 +1591,16 @@
         <v>38</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1589,16 +1611,16 @@
         <v>38</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1609,16 +1631,16 @@
         <v>38</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>51</v>
+        <v>133</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1629,16 +1651,16 @@
         <v>38</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1649,16 +1671,16 @@
         <v>38</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1669,16 +1691,16 @@
         <v>38</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1689,16 +1711,16 @@
         <v>38</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>51</v>
+        <v>133</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -1709,16 +1731,16 @@
         <v>38</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -1729,16 +1751,16 @@
         <v>38</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -1749,137 +1771,138 @@
         <v>38</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B35" s="2">
         <v>34</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B36" s="2">
         <v>35</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B37" s="2">
         <v>36</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B38" s="2">
         <v>37</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E38" s="2" t="s">
+      <c r="B39" s="2">
+        <v>38</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B39" s="2">
-        <v>38</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B40" s="2">
         <v>39</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1887,248 +1910,248 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFADAED-E972-4040-9C01-04C0703EB5D7}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
-    <col min="3" max="3" width="31.1640625" customWidth="1"/>
-    <col min="4" max="4" width="47.83203125" customWidth="1"/>
+    <col min="2" max="2" width="27.625" customWidth="1"/>
+    <col min="3" max="3" width="31.125" customWidth="1"/>
+    <col min="4" max="4" width="47.875" customWidth="1"/>
     <col min="5" max="5" width="61" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="E4" s="9">
         <v>12</v>
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="E5" s="9">
         <v>9</v>
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>3</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="E6" s="9">
         <v>7.5</v>
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>4</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="E7" s="9">
         <v>5.9</v>
       </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>5</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="E8" s="9">
         <v>4.0999999999999996</v>
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>6</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="E9" s="9">
         <v>3.5</v>
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>7</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="E10" s="9">
         <v>2</v>
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>8</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="E11" s="9">
         <v>1.7</v>
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>9</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="E12" s="9">
         <v>1.5</v>
       </c>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>10</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="E13" s="9">
         <v>1.2</v>
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -2136,7 +2159,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -2144,7 +2167,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2152,219 +2175,219 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>1</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="E21" s="9">
         <v>58214</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>2</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="E22" s="9">
         <v>51509</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>3</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="E23" s="9">
         <v>16998</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>4</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="E24" s="9">
         <v>11268</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>5</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="E25" s="9">
         <v>8776</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>6</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="E26" s="9">
         <v>5323</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>7</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="E27" s="9">
         <v>2485</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>8</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="E28" s="9">
         <v>2143</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>9</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="E29" s="9">
         <v>1781</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>10</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="E30" s="9">
         <v>1406</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>